<commit_message>
Add product duration and AM/PM application time to skincare selection
- Add duration_days and when_to_apply fields to Universkin products
- Create database migration for new columns (016_add_universkin_duration_and_apply_time.sql)
- Add AM/PM selector with Sun/Moon icons in SelectedProductCard
- Show total routine duration in estimated total card (shortest product)
- Add ImageLightbox component for full-screen product image preview
- Make product images clickable in both card and modal views
- Update header with centered premium icon and patient name subtitle
- Fix selector heights for consistent UI (Qty, Apply, Duration)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/design/universkin_products.xlsx
+++ b/design/universkin_products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\harlfoxem\AlmaUniverse\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6160F1DC-346D-4EDE-88C5-64430FE8238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C893C3-69BB-4AEC-B648-68FB1BBA0C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63795" yWindow="3150" windowWidth="15555" windowHeight="9060" xr2:uid="{7E574317-705C-4A8D-BCE8-7A2102288900}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{7E574317-705C-4A8D-BCE8-7A2102288900}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>Cleanse</t>
   </si>
@@ -153,6 +153,30 @@
   </si>
   <si>
     <t>price (usd)</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>60 days</t>
+  </si>
+  <si>
+    <t>90 days</t>
+  </si>
+  <si>
+    <t>30 days</t>
+  </si>
+  <si>
+    <t>when to apply</t>
+  </si>
+  <si>
+    <t>AM&amp;PM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>AM</t>
   </si>
 </sst>
 </file>
@@ -547,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E43EE6-CD3C-4CEB-8137-5EF1D2ABAFF4}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -558,7 +582,7 @@
     <col min="2" max="2" width="25.52734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -574,8 +598,14 @@
       <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -591,8 +621,14 @@
       <c r="E2">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -608,8 +644,14 @@
       <c r="E3">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -625,8 +667,14 @@
       <c r="E4">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -642,8 +690,14 @@
       <c r="E5">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -659,8 +713,14 @@
       <c r="E6">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -676,8 +736,14 @@
       <c r="E7">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -693,8 +759,14 @@
       <c r="E8">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -710,8 +782,14 @@
       <c r="E9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -727,8 +805,14 @@
       <c r="E10">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -744,8 +828,14 @@
       <c r="E11">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -761,8 +851,14 @@
       <c r="E12">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -777,6 +873,12 @@
       </c>
       <c r="E13">
         <v>75</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>